<commit_message>
Add support for saving results in PDF and update query input method
</commit_message>
<xml_diff>
--- a/articles.xlsx
+++ b/articles.xlsx
@@ -28,19 +28,6 @@
     <t>Citations</t>
   </si>
   <si>
-    <t>Machine learning for microbiologists</t>
-  </si>
-  <si>
-    <t>F Asnicar, AM Thomas, A Passerini… - Nature Reviews …, 2024 - nature.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">… how to evaluate a machine learning model and how … machine learning-based work. The 
-topics presented in this work will allow microbiologists to grasp the potential of machine learning …</t>
-  </si>
-  <si>
-    <t>https://www.nature.com/articles/s41579-023-00984-1</t>
-  </si>
-  <si>
     <t>Machine learning</t>
   </si>
   <si>
@@ -51,7 +38,7 @@
 popular machine learning … cover the core topics of machine learning in one semester, and …</t>
   </si>
   <si>
-    <t>https://books.google.com/books?hl=pt-PT&amp;lr=&amp;id=ctM-EAAAQBAJ&amp;oi=fnd&amp;pg=PR6&amp;dq=machine+learning&amp;ots=o_JpS6Ss0s&amp;sig=-4J9fzsu9PboZqXP-myzReu6jwE</t>
+    <t>https://books.google.com/books?hl=pt-PT&amp;lr=&amp;id=ctM-EAAAQBAJ&amp;oi=fnd&amp;pg=PR6&amp;dq=machine+learning&amp;ots=o_JpS9Uv3t&amp;sig=_C1-468zR4B8LkWxsHmgutop3Hs</t>
   </si>
   <si>
     <t>Quantum machine learning</t>
@@ -80,6 +67,19 @@
     <t>https://ieeexplore.ieee.org/abstract/document/8697857/</t>
   </si>
   <si>
+    <t>Machine learning algorithms-a review</t>
+  </si>
+  <si>
+    <t>B Mahesh - International Journal of Science and Research (IJSR) …, 2020 - researchgate.net</t>
+  </si>
+  <si>
+    <t xml:space="preserve">… Here‟sa quick look at some of the commonly used algorithms in machine learning (ML) 
+Supervised Learning Supervised learning is the machine learning task of learning a function …</t>
+  </si>
+  <si>
+    <t>https://www.researchgate.net/profile/Batta-Mahesh/publication/344717762_Machine_Learning_Algorithms_-A_Review/links/5f8b2365299bf1b53e2d243a/Machine-Learning-Algorithms-A-Review.pdf?eid=5082902844932096</t>
+  </si>
+  <si>
     <t>E Alpaydin - 2021 - books.google.com</t>
   </si>
   <si>
@@ -87,7 +87,7 @@
 of such applications as voice recognition and driverless cars. Today, machine learning …</t>
   </si>
   <si>
-    <t>https://books.google.com/books?hl=pt-PT&amp;lr=&amp;id=2nQJEAAAQBAJ&amp;oi=fnd&amp;pg=PR7&amp;dq=machine+learning&amp;ots=fI_aO8Vzls&amp;sig=4YqfAQ6oA17IuS_sqABqYRoHSPw</t>
+    <t>https://books.google.com/books?hl=pt-PT&amp;lr=&amp;id=2nQJEAAAQBAJ&amp;oi=fnd&amp;pg=PR7&amp;dq=machine+learning&amp;ots=fI_aObXCot&amp;sig=deL_-72Uy1QXyJ-BiXFA5f4H6vA</t>
   </si>
   <si>
     <t>What is machine learning?</t>
@@ -152,7 +152,7 @@
 are closely related to lifelong learning, most notably, multi-task learning and transfer learning, …</t>
   </si>
   <si>
-    <t>https://books.google.com/books?hl=pt-PT&amp;lr=&amp;id=z4RyEAAAQBAJ&amp;oi=fnd&amp;pg=PR1&amp;dq=machine+learning&amp;ots=r_cibe4xwF&amp;sig=AVpQDgEywws_exPhX00842l9yc4</t>
+    <t>https://books.google.com/books?hl=pt-PT&amp;lr=&amp;id=z4RyEAAAQBAJ&amp;oi=fnd&amp;pg=PR1&amp;dq=machine+learning&amp;ots=r_cibh6AzG&amp;sig=2izzu3LiJXIwlsTL8xs--fy7CGA</t>
   </si>
   <si>
     <t>Deep learning</t>
@@ -179,7 +179,7 @@
 conceptual background, deep learning techniques used in industry, and research perspectives.“…</t>
   </si>
   <si>
-    <t>https://books.google.com/books?hl=pt-PT&amp;lr=&amp;id=omivDQAAQBAJ&amp;oi=fnd&amp;pg=PR5&amp;dq=+deep+learning&amp;ots=MON69snBSX&amp;sig=HwCM7Jxs-64eFcgKVBnWblgIMGY</t>
+    <t>https://books.google.com/books?hl=pt-PT&amp;lr=&amp;id=omivDQAAQBAJ&amp;oi=fnd&amp;pg=PR5&amp;dq=+deep+learning&amp;ots=MON69vpEVZ&amp;sig=cO7lZp_UhCN7xX_nvTeoplMA12s</t>
   </si>
   <si>
     <t>N Rusk - Nature Methods, 2016 - nature.com</t>
@@ -199,7 +199,7 @@
 vision, speech recognition, machine translation, and driverless cars. Deep learning is an …</t>
   </si>
   <si>
-    <t>https://books.google.com/books?hl=pt-PT&amp;lr=&amp;id=b06qDwAAQBAJ&amp;oi=fnd&amp;pg=PP9&amp;dq=+deep+learning&amp;ots=_pA_OOjUYS&amp;sig=FvIKnfoEMFcxiIWtTJGHmLCJTMU</t>
+    <t>https://books.google.com/books?hl=pt-PT&amp;lr=&amp;id=b06qDwAAQBAJ&amp;oi=fnd&amp;pg=PP9&amp;dq=+deep+learning&amp;ots=_pA_ORlX-U&amp;sig=AP-l_990UVjeOSfKe6l_5HbrQTs</t>
   </si>
   <si>
     <t>Deep learning in bioinformatics</t>
@@ -725,7 +725,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>21</v>
@@ -844,16 +844,16 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C15" t="s">
         <v>48</v>
       </c>
       <c r="D15" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E15">
         <v>0</v>

</xml_diff>